<commit_message>
add column for metric 1&2
</commit_message>
<xml_diff>
--- a/Correlation/Metric 1, 2 and 3/commons-codec/Metric1,2&3_CommonsCodec.xlsx
+++ b/Correlation/Metric 1, 2 and 3/commons-codec/Metric1,2&3_CommonsCodec.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Classes\Ms Software Eng\6611 Software Measurement\Project\Correlation 1,2&amp;3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Measurement-Project\Correlation\Metric 1, 2 and 3\commons-codec\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8955" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8955"/>
   </bookViews>
   <sheets>
     <sheet name="CommonsCodec 1&amp;3" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="78">
   <si>
     <t>GROUP</t>
   </si>
@@ -253,12 +253,18 @@
   </si>
   <si>
     <t>Rule</t>
+  </si>
+  <si>
+    <t>Statement Coverage</t>
+  </si>
+  <si>
+    <t>Branch Coverage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -570,19 +576,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="1" max="1" width="0.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="0.85546875" customWidth="1"/>
+    <col min="5" max="13" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" customWidth="1"/>
+    <col min="15" max="15" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,8 +636,11 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -669,8 +683,12 @@
       <c r="N2">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <f>G2/(F2+G2)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -713,8 +731,12 @@
       <c r="N3">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <f t="shared" ref="O3:O50" si="0">G3/(F3+G3)*100</f>
+        <v>98.571428571428584</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -757,8 +779,12 @@
       <c r="N4">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>91.095890410958901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -801,8 +827,12 @@
       <c r="N5">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>94.117647058823522</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -845,8 +875,12 @@
       <c r="N6">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -889,8 +923,12 @@
       <c r="N7">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>85.227272727272734</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -933,8 +971,12 @@
       <c r="N8">
         <v>95</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -977,8 +1019,12 @@
       <c r="N9">
         <v>89</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>92.857142857142861</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1021,8 +1067,12 @@
       <c r="N10">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>91.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1065,8 +1115,12 @@
       <c r="N11">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1109,8 +1163,12 @@
       <c r="N12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1153,8 +1211,12 @@
       <c r="N13">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1197,8 +1259,12 @@
       <c r="N14">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1241,8 +1307,12 @@
       <c r="N15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1285,8 +1355,12 @@
       <c r="N16">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1329,8 +1403,12 @@
       <c r="N17">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>90.476190476190482</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1373,8 +1451,12 @@
       <c r="N18">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1417,8 +1499,12 @@
       <c r="N19">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <f t="shared" si="0"/>
+        <v>96.428571428571431</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1426,43 +1512,47 @@
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E20">
-        <v>55</v>
+        <v>564</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>143</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M20">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="N20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1470,43 +1560,47 @@
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>84</v>
+        <v>437</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N21">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1514,43 +1608,47 @@
         <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D22">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>564</v>
+        <v>1215</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="H22">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>143</v>
+        <v>202</v>
       </c>
       <c r="J22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K22">
-        <v>123</v>
+        <v>60</v>
       </c>
       <c r="L22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M22">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="N22">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1558,43 +1656,47 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>437</v>
+        <v>8509</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1602,43 +1704,47 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1215</v>
+        <v>433</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>202</v>
+        <v>79</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="N24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1646,43 +1752,47 @@
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>8509</v>
+        <v>50</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N25">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1690,43 +1800,47 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>433</v>
+        <v>375</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="J26">
         <v>0</v>
       </c>
       <c r="K26">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N26">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1734,19 +1848,19 @@
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1758,7 +1872,7 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -1769,96 +1883,108 @@
       <c r="N27">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>163</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>24</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>39</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>33</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>21</v>
+      </c>
+      <c r="N28">
+        <v>97</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29">
+        <v>71</v>
+      </c>
+      <c r="E29">
+        <v>2625</v>
+      </c>
+      <c r="F29">
+        <v>11</v>
+      </c>
+      <c r="G29">
+        <v>66</v>
+      </c>
+      <c r="H29">
+        <v>8</v>
+      </c>
+      <c r="I29">
+        <v>167</v>
+      </c>
+      <c r="J29">
+        <v>12</v>
+      </c>
+      <c r="K29">
         <v>44</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>375</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>26</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>69</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>24</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>11</v>
-      </c>
-      <c r="N28">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>72</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>4</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>13</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>7</v>
-      </c>
       <c r="L29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="N29">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="0"/>
+        <v>85.714285714285708</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1866,43 +1992,47 @@
         <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>163</v>
+        <v>485</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="J30">
         <v>0</v>
       </c>
       <c r="K30">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="L30">
         <v>0</v>
       </c>
       <c r="M30">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="N30">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1910,43 +2040,47 @@
         <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D31">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>2625</v>
+        <v>153</v>
       </c>
       <c r="F31">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G31">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="H31">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="J31">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="K31">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="L31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="N31">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1954,43 +2088,47 @@
         <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E32">
-        <v>485</v>
+        <v>192</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I32">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K32">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="L32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M32">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="N32">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>96.875</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1998,43 +2136,47 @@
         <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E33">
-        <v>153</v>
+        <v>35</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G33">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I33">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K33">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N33">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="0"/>
+        <v>57.142857142857139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2042,43 +2184,47 @@
         <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D34">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>192</v>
+        <v>335</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I34">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="J34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K34">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="L34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M34">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="N34">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2086,43 +2232,47 @@
         <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D35">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>35</v>
+        <v>462</v>
       </c>
       <c r="F35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G35">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="H35">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I35">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="J35">
         <v>5</v>
       </c>
       <c r="K35">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="L35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="N35">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="0"/>
+        <v>92.64705882352942</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2130,263 +2280,287 @@
         <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E36">
-        <v>335</v>
+        <v>1924</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G36">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I36">
+        <v>149</v>
+      </c>
+      <c r="J36">
+        <v>8</v>
+      </c>
+      <c r="K36">
+        <v>73</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>27</v>
+      </c>
+      <c r="N36">
+        <v>91</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="0"/>
+        <v>93.137254901960787</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" t="s">
         <v>57</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <v>38</v>
-      </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-      <c r="M36">
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>21</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>4</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>100</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>24</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>8</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>4</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>3</v>
+      </c>
+      <c r="N38">
+        <v>100</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39">
         <v>13</v>
       </c>
-      <c r="N36">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37">
+      <c r="E39">
+        <v>512</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>80</v>
+      </c>
+      <c r="H39">
         <v>4</v>
       </c>
-      <c r="E37">
-        <v>462</v>
-      </c>
-      <c r="F37">
+      <c r="I39">
+        <v>119</v>
+      </c>
+      <c r="J39">
+        <v>4</v>
+      </c>
+      <c r="K39">
+        <v>62</v>
+      </c>
+      <c r="L39">
+        <v>2</v>
+      </c>
+      <c r="M39">
+        <v>23</v>
+      </c>
+      <c r="N39">
+        <v>94</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="0"/>
+        <v>97.560975609756099</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>432</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>72</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>88</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>51</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>15</v>
+      </c>
+      <c r="N40">
+        <v>92</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41">
+        <v>19</v>
+      </c>
+      <c r="E41">
+        <v>127</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>18</v>
+      </c>
+      <c r="H41">
         <v>5</v>
       </c>
-      <c r="G37">
-        <v>63</v>
-      </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-      <c r="I37">
-        <v>92</v>
-      </c>
-      <c r="J37">
-        <v>5</v>
-      </c>
-      <c r="K37">
-        <v>52</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <v>23</v>
-      </c>
-      <c r="N37">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38">
-        <v>30</v>
-      </c>
-      <c r="E38">
-        <v>1924</v>
-      </c>
-      <c r="F38">
-        <v>7</v>
-      </c>
-      <c r="G38">
-        <v>95</v>
-      </c>
-      <c r="H38">
-        <v>4</v>
-      </c>
-      <c r="I38">
-        <v>149</v>
-      </c>
-      <c r="J38">
-        <v>8</v>
-      </c>
-      <c r="K38">
-        <v>73</v>
-      </c>
-      <c r="L38">
-        <v>1</v>
-      </c>
-      <c r="M38">
-        <v>27</v>
-      </c>
-      <c r="N38">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39">
+      <c r="I41">
+        <v>39</v>
+      </c>
+      <c r="J41">
         <v>3</v>
       </c>
-      <c r="E39">
+      <c r="K41">
         <v>21</v>
       </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>2</v>
-      </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="I39">
-        <v>4</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-      <c r="K39">
-        <v>2</v>
-      </c>
-      <c r="L39">
-        <v>1</v>
-      </c>
-      <c r="M39">
-        <v>1</v>
-      </c>
-      <c r="N39">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D40">
-        <v>6</v>
-      </c>
-      <c r="E40">
-        <v>30</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>3</v>
-      </c>
-      <c r="I40">
-        <v>11</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40">
-        <v>2</v>
-      </c>
-      <c r="L40">
-        <v>1</v>
-      </c>
-      <c r="M40">
-        <v>2</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41">
-        <v>5</v>
-      </c>
-      <c r="E41">
-        <v>24</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-      <c r="G41">
-        <v>3</v>
-      </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41">
-        <v>8</v>
-      </c>
-      <c r="J41">
-        <v>2</v>
-      </c>
-      <c r="K41">
-        <v>4</v>
-      </c>
       <c r="L41">
         <v>1</v>
       </c>
       <c r="M41">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="N41">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -2394,43 +2568,47 @@
         <v>60</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D42">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E42">
-        <v>512</v>
+        <v>335</v>
       </c>
       <c r="F42">
         <v>2</v>
       </c>
       <c r="G42">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="H42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I42">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="J42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K42">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="L42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M42">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="N42">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="0"/>
+        <v>95.238095238095227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -2438,43 +2616,47 @@
         <v>60</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>432</v>
+        <v>32</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="J43">
         <v>0</v>
       </c>
       <c r="K43">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="L43">
         <v>0</v>
       </c>
       <c r="M43">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="N43">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -2482,43 +2664,47 @@
         <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D44">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E44">
-        <v>127</v>
+        <v>340</v>
       </c>
       <c r="F44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="H44">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I44">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="J44">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K44">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="L44">
         <v>1</v>
       </c>
       <c r="M44">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2526,175 +2712,191 @@
         <v>60</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D45">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E45">
-        <v>335</v>
+        <v>169</v>
       </c>
       <c r="F45">
         <v>2</v>
       </c>
       <c r="G45">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>38</v>
+      </c>
+      <c r="J45">
+        <v>2</v>
+      </c>
+      <c r="K45">
+        <v>11</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>4</v>
+      </c>
+      <c r="N45">
+        <v>83</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="0"/>
+        <v>88.888888888888886</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46">
+        <v>43</v>
+      </c>
+      <c r="E46">
+        <v>654</v>
+      </c>
+      <c r="F46">
+        <v>5</v>
+      </c>
+      <c r="G46">
+        <v>37</v>
+      </c>
+      <c r="H46">
         <v>7</v>
       </c>
-      <c r="I45">
-        <v>97</v>
-      </c>
-      <c r="J45">
-        <v>3</v>
-      </c>
-      <c r="K45">
-        <v>35</v>
-      </c>
-      <c r="L45">
-        <v>1</v>
-      </c>
-      <c r="M45">
-        <v>16</v>
-      </c>
-      <c r="N45">
+      <c r="I46">
+        <v>105</v>
+      </c>
+      <c r="J46">
+        <v>5</v>
+      </c>
+      <c r="K46">
+        <v>29</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>11</v>
+      </c>
+      <c r="N46">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" t="s">
-        <v>60</v>
-      </c>
-      <c r="C46" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>32</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>2</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
+      <c r="O46">
+        <f t="shared" si="0"/>
+        <v>88.095238095238088</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>109</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>28</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>12</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>10</v>
+      </c>
+      <c r="N47">
+        <v>88</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>113</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>12</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>25</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>12</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
         <v>6</v>
       </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
-      <c r="K46">
-        <v>4</v>
-      </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-      <c r="M46">
-        <v>3</v>
-      </c>
-      <c r="N46">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47">
-        <v>3</v>
-      </c>
-      <c r="E47">
-        <v>340</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>46</v>
-      </c>
-      <c r="H47">
-        <v>1</v>
-      </c>
-      <c r="I47">
-        <v>87</v>
-      </c>
-      <c r="J47">
-        <v>1</v>
-      </c>
-      <c r="K47">
-        <v>37</v>
-      </c>
-      <c r="L47">
-        <v>1</v>
-      </c>
-      <c r="M47">
-        <v>14</v>
-      </c>
-      <c r="N47">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" t="s">
-        <v>67</v>
-      </c>
-      <c r="D48">
-        <v>8</v>
-      </c>
-      <c r="E48">
-        <v>169</v>
-      </c>
-      <c r="F48">
-        <v>2</v>
-      </c>
-      <c r="G48">
-        <v>16</v>
-      </c>
-      <c r="H48">
-        <v>2</v>
-      </c>
-      <c r="I48">
-        <v>38</v>
-      </c>
-      <c r="J48">
-        <v>2</v>
-      </c>
-      <c r="K48">
-        <v>11</v>
-      </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-      <c r="M48">
-        <v>4</v>
-      </c>
       <c r="N48">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -2702,43 +2904,47 @@
         <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E49">
-        <v>48</v>
+        <v>206</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I49">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="J49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K49">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="L49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N49">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="0"/>
+        <v>88.461538461538453</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -2746,282 +2952,71 @@
         <v>68</v>
       </c>
       <c r="C50" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="E50">
-        <v>48</v>
+        <v>809</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="I50">
-        <v>8</v>
+        <v>162</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K50">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="L50">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M50">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="N50">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>68</v>
-      </c>
-      <c r="C51" t="s">
-        <v>71</v>
-      </c>
-      <c r="D51">
-        <v>43</v>
-      </c>
-      <c r="E51">
-        <v>654</v>
-      </c>
-      <c r="F51">
-        <v>5</v>
-      </c>
-      <c r="G51">
-        <v>37</v>
-      </c>
-      <c r="H51">
-        <v>7</v>
-      </c>
-      <c r="I51">
-        <v>105</v>
-      </c>
-      <c r="J51">
-        <v>5</v>
-      </c>
-      <c r="K51">
-        <v>29</v>
-      </c>
-      <c r="L51">
-        <v>1</v>
-      </c>
-      <c r="M51">
-        <v>11</v>
-      </c>
-      <c r="N51">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" t="s">
-        <v>72</v>
-      </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <v>109</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52">
-        <v>4</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="I52">
-        <v>28</v>
-      </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
-      <c r="K52">
-        <v>12</v>
-      </c>
-      <c r="L52">
-        <v>0</v>
-      </c>
-      <c r="M52">
-        <v>10</v>
-      </c>
-      <c r="N52">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" t="s">
-        <v>73</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>113</v>
-      </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-      <c r="G53">
-        <v>12</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <v>25</v>
-      </c>
-      <c r="J53">
-        <v>0</v>
-      </c>
-      <c r="K53">
-        <v>12</v>
-      </c>
-      <c r="L53">
-        <v>0</v>
-      </c>
-      <c r="M53">
-        <v>6</v>
-      </c>
-      <c r="N53">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" t="s">
-        <v>74</v>
-      </c>
-      <c r="D54">
-        <v>30</v>
-      </c>
-      <c r="E54">
-        <v>206</v>
-      </c>
-      <c r="F54">
-        <v>3</v>
-      </c>
-      <c r="G54">
         <v>23</v>
       </c>
-      <c r="H54">
-        <v>3</v>
-      </c>
-      <c r="I54">
-        <v>44</v>
-      </c>
-      <c r="J54">
-        <v>3</v>
-      </c>
-      <c r="K54">
-        <v>16</v>
-      </c>
-      <c r="L54">
-        <v>1</v>
-      </c>
-      <c r="M54">
-        <v>5</v>
-      </c>
-      <c r="N54">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>68</v>
-      </c>
-      <c r="C55" t="s">
-        <v>75</v>
-      </c>
-      <c r="D55">
-        <v>130</v>
-      </c>
-      <c r="E55">
-        <v>809</v>
-      </c>
-      <c r="F55">
-        <v>11</v>
-      </c>
-      <c r="G55">
-        <v>105</v>
-      </c>
-      <c r="H55">
-        <v>17</v>
-      </c>
-      <c r="I55">
-        <v>162</v>
-      </c>
-      <c r="J55">
-        <v>14</v>
-      </c>
-      <c r="K55">
-        <v>66</v>
-      </c>
-      <c r="L55">
-        <v>4</v>
-      </c>
-      <c r="M55">
-        <v>18</v>
-      </c>
-      <c r="N55">
-        <v>23</v>
+      <c r="O50">
+        <f t="shared" si="0"/>
+        <v>90.517241379310349</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="13" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3064,8 +3059,11 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3108,8 +3106,12 @@
       <c r="N2">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <f>I2/(H2+I2)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3152,8 +3154,12 @@
       <c r="N3">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <f t="shared" ref="O3:O55" si="0">I3/(H3+I3)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3196,8 +3202,12 @@
       <c r="N4">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>98.317307692307693</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3240,8 +3250,12 @@
       <c r="N5">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>94.915254237288138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3284,8 +3298,12 @@
       <c r="N6">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3328,8 +3346,12 @@
       <c r="N7">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>94.656488549618317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3372,8 +3394,12 @@
       <c r="N8">
         <v>95</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3416,8 +3442,12 @@
       <c r="N9">
         <v>89</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3460,8 +3490,12 @@
       <c r="N10">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>98.80952380952381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3504,8 +3538,12 @@
       <c r="N11">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3548,8 +3586,12 @@
       <c r="N12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -3592,8 +3634,12 @@
       <c r="N13">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3636,8 +3682,12 @@
       <c r="N14">
         <v>75</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3680,8 +3730,12 @@
       <c r="N15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3724,8 +3778,12 @@
       <c r="N16">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>81.05263157894737</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3768,8 +3826,12 @@
       <c r="N17">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>97.014925373134332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -3812,8 +3874,12 @@
       <c r="N18">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>74.285714285714292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -3856,8 +3922,12 @@
       <c r="N19">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <f t="shared" si="0"/>
+        <v>99.337748344370851</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -3900,8 +3970,12 @@
       <c r="N20">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -3944,8 +4018,12 @@
       <c r="N21">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -3988,8 +4066,12 @@
       <c r="N22">
         <v>93</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>95.973154362416096</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -4032,8 +4114,12 @@
       <c r="N23">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -4076,8 +4162,12 @@
       <c r="N24">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -4120,8 +4210,12 @@
       <c r="N25">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -4164,8 +4258,12 @@
       <c r="N26">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -4208,8 +4306,12 @@
       <c r="N27">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -4252,8 +4354,12 @@
       <c r="N28">
         <v>89</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -4296,8 +4402,12 @@
       <c r="N29">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -4340,8 +4450,12 @@
       <c r="N30">
         <v>97</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -4384,8 +4498,12 @@
       <c r="N31">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <f t="shared" si="0"/>
+        <v>95.428571428571431</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -4428,8 +4546,12 @@
       <c r="N32">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -4472,8 +4594,12 @@
       <c r="N33">
         <v>77</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -4516,8 +4642,12 @@
       <c r="N34">
         <v>84</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <f t="shared" si="0"/>
+        <v>93.478260869565219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -4560,8 +4690,12 @@
       <c r="N35">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <f t="shared" si="0"/>
+        <v>66.666666666666657</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -4604,8 +4738,12 @@
       <c r="N36">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -4648,8 +4786,12 @@
       <c r="N37">
         <v>86</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <f t="shared" si="0"/>
+        <v>97.872340425531917</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -4692,8 +4834,12 @@
       <c r="N38">
         <v>91</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <f t="shared" si="0"/>
+        <v>97.385620915032675</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -4736,8 +4882,12 @@
       <c r="N39">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -4780,8 +4930,12 @@
       <c r="N40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <f t="shared" si="0"/>
+        <v>78.571428571428569</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -4824,8 +4978,12 @@
       <c r="N41">
         <v>100</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41">
+        <f t="shared" si="0"/>
+        <v>88.888888888888886</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -4868,8 +5026,12 @@
       <c r="N42">
         <v>94</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <f t="shared" si="0"/>
+        <v>96.747967479674799</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -4912,8 +5074,12 @@
       <c r="N43">
         <v>92</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -4956,8 +5122,12 @@
       <c r="N44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <f t="shared" si="0"/>
+        <v>88.63636363636364</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -5000,8 +5170,12 @@
       <c r="N45">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45">
+        <f t="shared" si="0"/>
+        <v>93.269230769230774</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -5044,8 +5218,12 @@
       <c r="N46">
         <v>100</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -5088,8 +5266,12 @@
       <c r="N47">
         <v>97</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47">
+        <f t="shared" si="0"/>
+        <v>98.86363636363636</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -5132,8 +5314,12 @@
       <c r="N48">
         <v>83</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -5176,8 +5362,12 @@
       <c r="N49">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -5220,8 +5410,12 @@
       <c r="N50">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -5264,8 +5458,12 @@
       <c r="N51">
         <v>89</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <f t="shared" si="0"/>
+        <v>93.75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -5308,8 +5506,12 @@
       <c r="N52">
         <v>88</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -5352,8 +5554,12 @@
       <c r="N53">
         <v>74</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -5396,8 +5602,12 @@
       <c r="N54">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <f t="shared" si="0"/>
+        <v>93.61702127659575</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -5439,6 +5649,10 @@
       </c>
       <c r="N55">
         <v>23</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="0"/>
+        <v>90.502793296089393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>